<commit_message>
Use the hyflbz.xlsx to gather the industry
</commit_message>
<xml_diff>
--- a/src/resource/hyflbz.xlsx
+++ b/src/resource/hyflbz.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="新标准" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="新标准英文" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -3987,8 +3987,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="00"/>
-    <numFmt numFmtId="177" formatCode="000"/>
+    <numFmt numFmtId="164" formatCode="00"/>
+    <numFmt numFmtId="165" formatCode="000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -4247,15 +4247,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4264,22 +4264,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4294,11 +4294,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4308,16 +4308,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4329,13 +4329,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -4388,7 +4388,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4400,21 +4400,21 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4429,26 +4429,29 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="24" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -4722,7 +4725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4731,9 +4734,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -4878,883 +4883,872 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="74"/>
-      <c r="B17" s="75"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8">
+        <v>13</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="74"/>
-      <c r="B18" s="75"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8">
+        <v>14</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="22.5">
       <c r="A19" s="7"/>
       <c r="B19" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="7"/>
       <c r="B20" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="22.5">
-      <c r="A21" s="7"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="12"/>
       <c r="B21" s="8">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="7"/>
       <c r="B22" s="8">
-        <v>16</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="12"/>
       <c r="B23" s="8">
-        <v>17</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="33.75">
+      <c r="A24" s="12"/>
       <c r="B24" s="8">
-        <v>18</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="12"/>
       <c r="B25" s="8">
-        <v>19</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="33.75">
+        <v>21</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="12"/>
       <c r="B26" s="8">
-        <v>20</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="22.5">
       <c r="A27" s="12"/>
       <c r="B27" s="8">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="33.75">
       <c r="A28" s="12"/>
       <c r="B28" s="8">
-        <v>22</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="22.5">
       <c r="A29" s="12"/>
       <c r="B29" s="8">
-        <v>23</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="33.75">
+        <v>25</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="22.5">
       <c r="A30" s="12"/>
       <c r="B30" s="8">
-        <v>24</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="22.5">
-      <c r="A31" s="12"/>
+        <v>26</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="7"/>
       <c r="B31" s="8">
-        <v>25</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="22.5">
-      <c r="A32" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="7"/>
       <c r="B32" s="8">
-        <v>26</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="22.5">
+      <c r="A33" s="12"/>
       <c r="B33" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="7"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="22.5">
+      <c r="A34" s="12"/>
       <c r="B34" s="8">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="22.5">
       <c r="A35" s="12"/>
       <c r="B35" s="8">
-        <v>29</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>124</v>
+        <v>31</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="22.5">
       <c r="A36" s="12"/>
       <c r="B36" s="8">
-        <v>30</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="22.5">
+        <v>32</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="12"/>
       <c r="B37" s="8">
-        <v>31</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="22.5">
+        <v>33</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="12"/>
       <c r="B38" s="8">
-        <v>32</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="12"/>
       <c r="B39" s="8">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="12"/>
       <c r="B40" s="8">
-        <v>34</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="8">
-        <v>35</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>36</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="33.75">
+      <c r="A41" s="7"/>
+      <c r="B41" s="10">
+        <v>37</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="22.5">
       <c r="A42" s="12"/>
       <c r="B42" s="8">
-        <v>36</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="33.75">
       <c r="A43" s="7"/>
-      <c r="B43" s="10">
-        <v>37</v>
-      </c>
-      <c r="C43" s="21" t="s">
+      <c r="B43" s="8">
+        <v>39</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="8">
+        <v>40</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="8">
+        <v>41</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="23.25" thickBot="1">
+      <c r="A46" s="13"/>
+      <c r="B46" s="22">
+        <v>42</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="23.25" thickBot="1">
+      <c r="A47" s="7"/>
+      <c r="B47" s="17">
+        <v>43</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="81">
+      <c r="A48" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="24"/>
+    </row>
+    <row r="49" spans="1:6" ht="22.5">
+      <c r="A49" s="7"/>
+      <c r="B49" s="8">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="22.5">
-      <c r="A44" s="12"/>
-      <c r="B44" s="8">
-        <v>38</v>
-      </c>
-      <c r="C44" s="21" t="s">
+      <c r="C49" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="22.5">
+      <c r="A50" s="7"/>
+      <c r="B50" s="8">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="33.75">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8">
-        <v>39</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8">
-        <v>40</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="12"/>
-      <c r="B47" s="8">
-        <v>41</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="23.25" thickBot="1">
-      <c r="A48" s="13"/>
-      <c r="B48" s="22">
-        <v>42</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="23.25" thickBot="1">
-      <c r="A49" s="7"/>
-      <c r="B49" s="17">
-        <v>43</v>
-      </c>
-      <c r="C49" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="81">
-      <c r="A50" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="24"/>
+      <c r="C50" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="22.5">
       <c r="A51" s="7"/>
       <c r="B51" s="8">
-        <v>44</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="22.5">
-      <c r="A52" s="7"/>
-      <c r="B52" s="8">
-        <v>45</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="22.5">
-      <c r="A53" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="24"/>
+    </row>
+    <row r="53" spans="1:6" ht="19.5">
+      <c r="A53" s="14"/>
       <c r="B53" s="8">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="24"/>
+        <v>125</v>
+      </c>
+      <c r="E53" s="32"/>
+      <c r="F53" s="33"/>
+    </row>
+    <row r="54" spans="1:6" ht="19.5">
+      <c r="A54" s="14"/>
+      <c r="B54" s="8">
+        <v>48</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="32"/>
+      <c r="F54" s="33"/>
     </row>
     <row r="55" spans="1:6" ht="19.5">
       <c r="A55" s="14"/>
       <c r="B55" s="8">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E55" s="32"/>
       <c r="F55" s="33"/>
     </row>
-    <row r="56" spans="1:6" ht="19.5">
+    <row r="56" spans="1:6" ht="22.5">
       <c r="A56" s="14"/>
       <c r="B56" s="8">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E56" s="32"/>
       <c r="F56" s="33"/>
     </row>
-    <row r="57" spans="1:6" ht="19.5">
-      <c r="A57" s="14"/>
-      <c r="B57" s="8">
-        <v>49</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>127</v>
-      </c>
+    <row r="57" spans="1:6" ht="22.5">
+      <c r="A57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="11"/>
       <c r="E57" s="32"/>
       <c r="F57" s="33"/>
     </row>
-    <row r="58" spans="1:6" ht="22.5">
-      <c r="A58" s="14"/>
-      <c r="B58" s="8">
-        <v>50</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E58" s="32"/>
-      <c r="F58" s="33"/>
-    </row>
-    <row r="59" spans="1:6" ht="22.5">
-      <c r="A59" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="11"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="33"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="7"/>
-      <c r="B60" s="25">
+    <row r="58" spans="1:6">
+      <c r="A58" s="7"/>
+      <c r="B58" s="25">
         <v>51</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C58" s="26" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="27"/>
+      <c r="B59" s="8">
+        <v>52</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="54">
+      <c r="A60" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="24"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="27"/>
       <c r="B61" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="54">
-      <c r="A62" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="24"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="7"/>
+      <c r="B62" s="8">
+        <v>54</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="27"/>
       <c r="B63" s="8">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="7"/>
+      <c r="A64" s="27"/>
       <c r="B64" s="8">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="27"/>
       <c r="B65" s="8">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="27"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="22.5">
+      <c r="A66" s="12"/>
       <c r="B66" s="8">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="27"/>
       <c r="B67" s="8">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="22.5">
-      <c r="A68" s="12"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="27"/>
       <c r="B68" s="8">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="27"/>
-      <c r="B69" s="8">
-        <v>59</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="27">
+      <c r="A69" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="27"/>
       <c r="B70" s="8">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="27">
-      <c r="A71" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="27"/>
-      <c r="B72" s="8">
-        <v>61</v>
-      </c>
-      <c r="C72" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="71" spans="1:3">
+      <c r="A71" s="12"/>
+      <c r="B71" s="8">
+        <v>62</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="67.5">
+      <c r="A72" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" s="24"/>
+    </row>
+    <row r="73" spans="1:3" ht="22.5">
       <c r="A73" s="12"/>
       <c r="B73" s="8">
-        <v>62</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="67.5">
-      <c r="A74" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C74" s="24"/>
+        <v>63</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="22.5">
+      <c r="A74" s="7"/>
+      <c r="B74" s="17">
+        <v>64</v>
+      </c>
+      <c r="C74" s="28" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="22.5">
-      <c r="A75" s="12"/>
+      <c r="A75" s="27"/>
       <c r="B75" s="8">
-        <v>63</v>
-      </c>
-      <c r="C75" s="21" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="22.5">
-      <c r="A76" s="7"/>
-      <c r="B76" s="17">
-        <v>64</v>
-      </c>
-      <c r="C76" s="28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="22.5">
+        <v>65</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C76" s="24"/>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="27"/>
       <c r="B77" s="8">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" s="24"/>
+      <c r="A78" s="12"/>
+      <c r="B78" s="8">
+        <v>67</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="27"/>
       <c r="B79" s="8">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="12"/>
       <c r="B80" s="8">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="27"/>
-      <c r="B81" s="8">
-        <v>68</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>86</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="27">
+      <c r="A81" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81" s="24"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="12"/>
+      <c r="A82" s="27"/>
       <c r="B82" s="8">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="27">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="40.5">
       <c r="A83" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>89</v>
+        <v>1051</v>
       </c>
       <c r="C83" s="24"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="27"/>
       <c r="B84" s="8">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="40.5">
-      <c r="A85" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C85" s="24"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="27"/>
-      <c r="B86" s="8">
-        <v>71</v>
-      </c>
-      <c r="C86" s="9" t="s">
         <v>92</v>
       </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="27"/>
+      <c r="B85" s="8">
+        <v>72</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="54">
+      <c r="A86" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="24"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="27"/>
       <c r="B87" s="8">
-        <v>72</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="54">
-      <c r="A88" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B88" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C88" s="24"/>
+        <v>73</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="27"/>
+      <c r="B88" s="8">
+        <v>74</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="27"/>
+      <c r="A89" s="7"/>
       <c r="B89" s="8">
-        <v>73</v>
-      </c>
-      <c r="C89" s="21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="27"/>
-      <c r="B90" s="8">
-        <v>74</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>97</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="67.5">
+      <c r="A90" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90" s="24"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="7"/>
+      <c r="A91" s="12"/>
       <c r="B91" s="8">
-        <v>75</v>
-      </c>
-      <c r="C91" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="67.5">
-      <c r="A92" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C92" s="24"/>
+        <v>76</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="22.5">
+      <c r="A92" s="12"/>
+      <c r="B92" s="8">
+        <v>77</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="12"/>
       <c r="B93" s="8">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="22.5">
-      <c r="A94" s="12"/>
-      <c r="B94" s="8">
-        <v>77</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>102</v>
-      </c>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="67.5">
+      <c r="A94" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C94" s="29"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="12"/>
-      <c r="B95" s="8">
-        <v>78</v>
+      <c r="B95" s="25">
+        <v>79</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="67.5">
-      <c r="A96" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C96" s="29"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="33.75">
+      <c r="A96" s="27"/>
+      <c r="B96" s="8">
+        <v>80</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="12"/>
-      <c r="B97" s="25">
-        <v>79</v>
+      <c r="A97" s="7"/>
+      <c r="B97" s="17">
+        <v>81</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="33.75">
-      <c r="A98" s="27"/>
-      <c r="B98" s="8">
-        <v>80</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>107</v>
-      </c>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C98" s="24"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="7"/>
-      <c r="B99" s="17">
-        <v>81</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="A99" s="30"/>
+      <c r="B99" s="25">
+        <v>82</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="40.5">
       <c r="A100" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>110</v>
+        <v>1052</v>
       </c>
       <c r="C100" s="24"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="30"/>
-      <c r="B101" s="25">
-        <v>82</v>
-      </c>
-      <c r="C101" s="21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="40.5">
-      <c r="A102" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B102" s="15" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C102" s="24"/>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="27"/>
-      <c r="B103" s="8">
+      <c r="A101" s="27"/>
+      <c r="B101" s="8">
         <v>83</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C101" s="9" t="s">
         <v>113</v>
       </c>
     </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="27"/>
+      <c r="B102" s="8">
+        <v>84</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="40.5">
+      <c r="A103" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C103" s="24"/>
+    </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="27"/>
+      <c r="A104" s="12"/>
       <c r="B104" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="40.5">
-      <c r="A105" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B105" s="15" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C105" s="24"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="33.75">
+      <c r="A105" s="12"/>
+      <c r="B105" s="8">
+        <v>86</v>
+      </c>
+      <c r="C105" s="21" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="12"/>
       <c r="B106" s="8">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="33.75">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" s="12"/>
       <c r="B107" s="8">
-        <v>86</v>
-      </c>
-      <c r="C107" s="21" t="s">
-        <v>118</v>
+        <v>88</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="12"/>
       <c r="B108" s="8">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="12"/>
-      <c r="B109" s="8">
-        <v>88</v>
-      </c>
-      <c r="C109" s="9" t="s">
-        <v>120</v>
-      </c>
+      <c r="A109" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C109" s="24"/>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="12"/>
       <c r="B110" s="8">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C111" s="24"/>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="B112" s="8">
-        <v>90</v>
-      </c>
-      <c r="C112" s="9" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
@@ -8980,10 +8974,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9128,884 +9122,872 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" ht="15" customHeight="1">
       <c r="A16" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="75" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="74"/>
-      <c r="B17" s="76"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="74"/>
-      <c r="B18" s="76"/>
+    <row r="17" spans="1:3" ht="25.5">
+      <c r="A17" s="7"/>
+      <c r="B17" s="61">
+        <v>13</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="25.5">
+      <c r="A18" s="7"/>
+      <c r="B18" s="61">
+        <v>14</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>1069</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="25.5">
       <c r="A19" s="7"/>
       <c r="B19" s="61">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="25.5">
       <c r="A20" s="7"/>
       <c r="B20" s="61">
-        <v>14</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="25.5">
-      <c r="A21" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25">
+      <c r="A21" s="12"/>
       <c r="B21" s="61">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="25.5">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="7"/>
       <c r="B22" s="61">
-        <v>16</v>
-      </c>
-      <c r="C22" s="66" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25">
+        <v>18</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="51">
       <c r="A23" s="12"/>
       <c r="B23" s="61">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="7"/>
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="63.75">
+      <c r="A24" s="12"/>
       <c r="B24" s="61">
-        <v>18</v>
-      </c>
-      <c r="C24" s="56" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="51">
+        <v>20</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="25.5">
       <c r="A25" s="12"/>
       <c r="B25" s="61">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C25" s="65" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="63.75">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="38.25">
       <c r="A26" s="12"/>
       <c r="B26" s="61">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C26" s="65" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="25.5">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25">
       <c r="A27" s="12"/>
       <c r="B27" s="61">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C27" s="65" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="38.25">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="51">
       <c r="A28" s="12"/>
       <c r="B28" s="61">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.25">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="25.5">
       <c r="A29" s="12"/>
       <c r="B29" s="61">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C29" s="65" t="s">
-        <v>1078</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="51">
       <c r="A30" s="12"/>
       <c r="B30" s="61">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="25.5">
-      <c r="A31" s="12"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="61">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C31" s="65" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="51">
-      <c r="A32" s="12"/>
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="25.5">
+      <c r="A32" s="7"/>
       <c r="B32" s="61">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C32" s="65" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="25.5">
-      <c r="A33" s="7"/>
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="38.25">
+      <c r="A33" s="12"/>
       <c r="B33" s="61">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C33" s="65" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="25.5">
-      <c r="A34" s="7"/>
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="38.25">
+      <c r="A34" s="12"/>
       <c r="B34" s="61">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C34" s="65" t="s">
-        <v>1125</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="38.25">
       <c r="A35" s="12"/>
       <c r="B35" s="61">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C35" s="65" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="38.25">
       <c r="A36" s="12"/>
       <c r="B36" s="61">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="38.25">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.25">
       <c r="A37" s="12"/>
       <c r="B37" s="61">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C37" s="65" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="38.25">
       <c r="A38" s="12"/>
       <c r="B38" s="61">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C38" s="65" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="38.25">
       <c r="A39" s="12"/>
       <c r="B39" s="61">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C39" s="65" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="38.25">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.25">
       <c r="A40" s="12"/>
       <c r="B40" s="61">
-        <v>34</v>
-      </c>
-      <c r="C40" s="65" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="38.25">
-      <c r="A41" s="12"/>
+        <v>36</v>
+      </c>
+      <c r="C40" s="67" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="76.5">
+      <c r="A41" s="7"/>
       <c r="B41" s="61">
-        <v>35</v>
-      </c>
-      <c r="C41" s="65" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25">
+        <v>37</v>
+      </c>
+      <c r="C41" s="68" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="51">
       <c r="A42" s="12"/>
       <c r="B42" s="61">
-        <v>36</v>
-      </c>
-      <c r="C42" s="67" t="s">
-        <v>1087</v>
+        <v>38</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>1128</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="76.5">
       <c r="A43" s="7"/>
       <c r="B43" s="61">
-        <v>37</v>
-      </c>
-      <c r="C43" s="68" t="s">
-        <v>1127</v>
+        <v>39</v>
+      </c>
+      <c r="C43" s="66" t="s">
+        <v>1129</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="51">
-      <c r="A44" s="12"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="61">
-        <v>38</v>
-      </c>
-      <c r="C44" s="65" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="76.5">
-      <c r="A45" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C44" s="68" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="25.5">
+      <c r="A45" s="12"/>
       <c r="B45" s="61">
-        <v>39</v>
-      </c>
-      <c r="C45" s="66" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="51">
-      <c r="A46" s="7"/>
-      <c r="B46" s="61">
-        <v>40</v>
-      </c>
-      <c r="C46" s="68" t="s">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="25.5">
-      <c r="A47" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="C45" s="65" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="51.75" thickBot="1">
+      <c r="A46" s="13"/>
+      <c r="B46" s="69">
+        <v>42</v>
+      </c>
+      <c r="C46" s="70" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="39" thickBot="1">
+      <c r="A47" s="7"/>
       <c r="B47" s="61">
-        <v>41</v>
-      </c>
-      <c r="C47" s="65" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A48" s="13"/>
-      <c r="B48" s="69">
-        <v>42</v>
-      </c>
-      <c r="C48" s="70" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="39" thickBot="1">
+        <v>43</v>
+      </c>
+      <c r="C47" s="70" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="62" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C48" s="71"/>
+    </row>
+    <row r="49" spans="1:6" ht="51">
       <c r="A49" s="7"/>
       <c r="B49" s="61">
-        <v>43</v>
-      </c>
-      <c r="C49" s="70" t="s">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="62" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C50" s="71"/>
-    </row>
-    <row r="51" spans="1:6" ht="51">
+        <v>44</v>
+      </c>
+      <c r="C49" s="65" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="25.5">
+      <c r="A50" s="7"/>
+      <c r="B50" s="61">
+        <v>45</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="38.25">
       <c r="A51" s="7"/>
       <c r="B51" s="61">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C51" s="65" t="s">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="25.5">
-      <c r="A52" s="7"/>
-      <c r="B52" s="61">
-        <v>45</v>
-      </c>
-      <c r="C52" s="65" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="38.25">
-      <c r="A53" s="7"/>
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="62" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C52" s="71"/>
+    </row>
+    <row r="53" spans="1:6" ht="19.5">
+      <c r="A53" s="14"/>
       <c r="B53" s="61">
-        <v>46</v>
-      </c>
-      <c r="C53" s="65" t="s">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="62" t="s">
-        <v>1092</v>
-      </c>
-      <c r="C54" s="71"/>
+        <v>47</v>
+      </c>
+      <c r="C53" s="67" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E53" s="32"/>
+      <c r="F53" s="33"/>
+    </row>
+    <row r="54" spans="1:6" ht="38.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="61">
+        <v>48</v>
+      </c>
+      <c r="C54" s="65" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E54" s="32"/>
+      <c r="F54" s="33"/>
     </row>
     <row r="55" spans="1:6" ht="19.5">
       <c r="A55" s="14"/>
       <c r="B55" s="61">
-        <v>47</v>
-      </c>
-      <c r="C55" s="67" t="s">
-        <v>1093</v>
+        <v>49</v>
+      </c>
+      <c r="C55" s="57" t="s">
+        <v>1121</v>
       </c>
       <c r="E55" s="32"/>
       <c r="F55" s="33"/>
     </row>
-    <row r="56" spans="1:6" ht="38.25">
+    <row r="56" spans="1:6" ht="51">
       <c r="A56" s="14"/>
       <c r="B56" s="61">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C56" s="65" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="E56" s="32"/>
       <c r="F56" s="33"/>
     </row>
-    <row r="57" spans="1:6" ht="19.5">
-      <c r="A57" s="14"/>
-      <c r="B57" s="61">
-        <v>49</v>
-      </c>
-      <c r="C57" s="57" t="s">
-        <v>1121</v>
-      </c>
+    <row r="57" spans="1:6" ht="25.5">
+      <c r="A57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="66" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C57" s="71"/>
       <c r="E57" s="32"/>
       <c r="F57" s="33"/>
     </row>
-    <row r="58" spans="1:6" ht="51">
-      <c r="A58" s="14"/>
-      <c r="B58" s="61">
-        <v>50</v>
-      </c>
-      <c r="C58" s="65" t="s">
-        <v>1136</v>
-      </c>
-      <c r="E58" s="32"/>
-      <c r="F58" s="33"/>
-    </row>
-    <row r="59" spans="1:6" ht="25.5">
-      <c r="A59" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" s="66" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C59" s="71"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="33"/>
-    </row>
-    <row r="60" spans="1:6" ht="14.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="64">
+    <row r="58" spans="1:6" ht="14.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="64">
         <v>51</v>
       </c>
-      <c r="C60" s="72" t="s">
+      <c r="C58" s="72" t="s">
         <v>1094</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="14.25">
+    <row r="59" spans="1:6" ht="14.25">
+      <c r="A59" s="27"/>
+      <c r="B59" s="61">
+        <v>52</v>
+      </c>
+      <c r="C59" s="66" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="25.5">
+      <c r="A60" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="65" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C60" s="71"/>
+    </row>
+    <row r="61" spans="1:6" ht="25.5">
       <c r="A61" s="27"/>
       <c r="B61" s="61">
-        <v>52</v>
-      </c>
-      <c r="C61" s="66" t="s">
-        <v>1095</v>
+        <v>53</v>
+      </c>
+      <c r="C61" s="65" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="25.5">
-      <c r="A62" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="65" t="s">
-        <v>1096</v>
-      </c>
-      <c r="C62" s="71"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="61">
+        <v>54</v>
+      </c>
+      <c r="C62" s="65" t="s">
+        <v>1097</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="25.5">
       <c r="A63" s="27"/>
       <c r="B63" s="61">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C63" s="65" t="s">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="25.5">
-      <c r="A64" s="7"/>
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="14.25">
+      <c r="A64" s="27"/>
       <c r="B64" s="61">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C64" s="65" t="s">
-        <v>1097</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="25.5">
       <c r="A65" s="27"/>
       <c r="B65" s="61">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C65" s="65" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.25">
-      <c r="A66" s="27"/>
+      <c r="A66" s="12"/>
       <c r="B66" s="61">
-        <v>56</v>
-      </c>
-      <c r="C66" s="65" t="s">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="25.5">
+        <v>58</v>
+      </c>
+      <c r="C66" s="67" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14.25">
       <c r="A67" s="27"/>
       <c r="B67" s="61">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C67" s="65" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="14.25">
-      <c r="A68" s="12"/>
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="27"/>
       <c r="B68" s="61">
-        <v>58</v>
-      </c>
-      <c r="C68" s="67" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="14.25">
-      <c r="A69" s="27"/>
-      <c r="B69" s="61">
-        <v>59</v>
-      </c>
-      <c r="C69" s="65" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>60</v>
+      </c>
+      <c r="C68" s="57" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="38.25">
+      <c r="A69" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="65" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C69" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14.25">
       <c r="A70" s="27"/>
       <c r="B70" s="61">
-        <v>60</v>
-      </c>
-      <c r="C70" s="57" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="38.25">
-      <c r="A71" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B71" s="65" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C71" s="71" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="14.25">
-      <c r="A72" s="27"/>
-      <c r="B72" s="61">
-        <v>61</v>
-      </c>
-      <c r="C72" s="65" t="s">
+      <c r="C70" s="65" t="s">
         <v>1103</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="25.5">
+    <row r="71" spans="1:3" ht="25.5">
+      <c r="A71" s="12"/>
+      <c r="B71" s="61">
+        <v>62</v>
+      </c>
+      <c r="C71" s="65" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="89.25">
+      <c r="A72" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" s="66" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C72" s="71"/>
+    </row>
+    <row r="73" spans="1:3" ht="63.75">
       <c r="A73" s="12"/>
       <c r="B73" s="61">
-        <v>62</v>
-      </c>
-      <c r="C73" s="65" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="89.25">
-      <c r="A74" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" s="66" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C74" s="71"/>
-    </row>
-    <row r="75" spans="1:3" ht="63.75">
-      <c r="A75" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="C73" s="68" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="25.5">
+      <c r="A74" s="7"/>
+      <c r="B74" s="61">
+        <v>64</v>
+      </c>
+      <c r="C74" s="66" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="51">
+      <c r="A75" s="27"/>
       <c r="B75" s="61">
-        <v>63</v>
-      </c>
-      <c r="C75" s="68" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="25.5">
-      <c r="A76" s="7"/>
-      <c r="B76" s="61">
-        <v>64</v>
-      </c>
-      <c r="C76" s="66" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="51">
+        <v>65</v>
+      </c>
+      <c r="C75" s="66" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="14.25">
+      <c r="A76" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" s="66" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C76" s="71"/>
+    </row>
+    <row r="77" spans="1:3" ht="25.5">
       <c r="A77" s="27"/>
       <c r="B77" s="61">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C77" s="66" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="14.25">
-      <c r="A78" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78" s="66" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C78" s="71"/>
-    </row>
-    <row r="79" spans="1:3" ht="25.5">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="25.5">
+      <c r="A78" s="12"/>
+      <c r="B78" s="61">
+        <v>67</v>
+      </c>
+      <c r="C78" s="66" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.25">
       <c r="A79" s="27"/>
       <c r="B79" s="61">
-        <v>66</v>
-      </c>
-      <c r="C79" s="66" t="s">
-        <v>1145</v>
+        <v>68</v>
+      </c>
+      <c r="C79" s="65" t="s">
+        <v>1105</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="25.5">
       <c r="A80" s="12"/>
       <c r="B80" s="61">
-        <v>67</v>
-      </c>
-      <c r="C80" s="66" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="14.25">
-      <c r="A81" s="27"/>
-      <c r="B81" s="61">
-        <v>68</v>
-      </c>
-      <c r="C81" s="65" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="25.5">
-      <c r="A82" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="C80" s="65" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" s="62" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C81" s="71"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="27"/>
       <c r="B82" s="61">
-        <v>69</v>
-      </c>
-      <c r="C82" s="65" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>70</v>
+      </c>
+      <c r="C82" s="62" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="51">
       <c r="A83" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B83" s="62" t="s">
-        <v>1107</v>
+        <v>90</v>
+      </c>
+      <c r="B83" s="65" t="s">
+        <v>1147</v>
       </c>
       <c r="C83" s="71"/>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" ht="14.25">
       <c r="A84" s="27"/>
       <c r="B84" s="61">
-        <v>70</v>
-      </c>
-      <c r="C84" s="62" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="51">
-      <c r="A85" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B85" s="65" t="s">
-        <v>1147</v>
-      </c>
-      <c r="C85" s="71"/>
-    </row>
-    <row r="86" spans="1:3" ht="14.25">
-      <c r="A86" s="27"/>
-      <c r="B86" s="61">
         <v>71</v>
       </c>
-      <c r="C86" s="66" t="s">
+      <c r="C84" s="66" t="s">
         <v>1108</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="25.5">
+    <row r="85" spans="1:3" ht="25.5">
+      <c r="A85" s="27"/>
+      <c r="B85" s="61">
+        <v>72</v>
+      </c>
+      <c r="C85" s="66" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="63.75">
+      <c r="A86" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="66" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C86" s="71"/>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="27"/>
       <c r="B87" s="61">
-        <v>72</v>
-      </c>
-      <c r="C87" s="66" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="63.75">
-      <c r="A88" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B88" s="66" t="s">
-        <v>1148</v>
-      </c>
-      <c r="C88" s="71"/>
+        <v>73</v>
+      </c>
+      <c r="C87" s="57" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="25.5">
+      <c r="A88" s="27"/>
+      <c r="B88" s="61">
+        <v>74</v>
+      </c>
+      <c r="C88" s="66" t="s">
+        <v>1150</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="27"/>
+      <c r="A89" s="7"/>
       <c r="B89" s="61">
-        <v>73</v>
-      </c>
-      <c r="C89" s="57" t="s">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="25.5">
-      <c r="A90" s="27"/>
-      <c r="B90" s="61">
-        <v>74</v>
-      </c>
-      <c r="C90" s="66" t="s">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="C89" s="56" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="102">
+      <c r="A90" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="66" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C90" s="71"/>
+    </row>
+    <row r="91" spans="1:3" ht="38.25">
+      <c r="A91" s="12"/>
       <c r="B91" s="61">
-        <v>75</v>
-      </c>
-      <c r="C91" s="56" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="102">
-      <c r="A92" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92" s="66" t="s">
-        <v>1152</v>
-      </c>
-      <c r="C92" s="71"/>
-    </row>
-    <row r="93" spans="1:3" ht="38.25">
+        <v>76</v>
+      </c>
+      <c r="C91" s="66" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="51">
+      <c r="A92" s="12"/>
+      <c r="B92" s="61">
+        <v>77</v>
+      </c>
+      <c r="C92" s="66" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="25.5">
       <c r="A93" s="12"/>
       <c r="B93" s="61">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C93" s="66" t="s">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="51">
-      <c r="A94" s="12"/>
-      <c r="B94" s="61">
-        <v>77</v>
-      </c>
-      <c r="C94" s="66" t="s">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="25.5">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="63.75">
+      <c r="A94" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B94" s="66" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C94" s="71"/>
+    </row>
+    <row r="95" spans="1:3" ht="14.25">
       <c r="A95" s="12"/>
-      <c r="B95" s="61">
-        <v>78</v>
+      <c r="B95" s="64">
+        <v>79</v>
       </c>
       <c r="C95" s="66" t="s">
-        <v>1110</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="63.75">
-      <c r="A96" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B96" s="66" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C96" s="71"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="61">
+        <v>80</v>
+      </c>
+      <c r="C96" s="66" t="s">
+        <v>1157</v>
+      </c>
     </row>
     <row r="97" spans="1:3" ht="14.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="64">
-        <v>79</v>
+      <c r="A97" s="7"/>
+      <c r="B97" s="61">
+        <v>81</v>
       </c>
       <c r="C97" s="66" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="63.75">
-      <c r="A98" s="27"/>
-      <c r="B98" s="61">
-        <v>80</v>
-      </c>
-      <c r="C98" s="66" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="14.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="61">
-        <v>81</v>
-      </c>
-      <c r="C99" s="66" t="s">
         <v>1111</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="98" spans="1:3">
+      <c r="A98" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B98" s="57" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C98" s="71"/>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="30"/>
+      <c r="B99" s="64">
+        <v>82</v>
+      </c>
+      <c r="C99" s="57" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="38.25">
       <c r="A100" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B100" s="57" t="s">
-        <v>1112</v>
+        <v>111</v>
+      </c>
+      <c r="B100" s="66" t="s">
+        <v>1158</v>
       </c>
       <c r="C100" s="71"/>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="30"/>
-      <c r="B101" s="64">
-        <v>82</v>
-      </c>
-      <c r="C101" s="57" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="38.25">
-      <c r="A102" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B102" s="66" t="s">
-        <v>1158</v>
-      </c>
-      <c r="C102" s="71"/>
-    </row>
-    <row r="103" spans="1:3" ht="14.25">
-      <c r="A103" s="27"/>
-      <c r="B103" s="61">
+    <row r="101" spans="1:3" ht="14.25">
+      <c r="A101" s="27"/>
+      <c r="B101" s="61">
         <v>83</v>
       </c>
-      <c r="C103" s="66" t="s">
+      <c r="C101" s="66" t="s">
         <v>1113</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="14.25">
-      <c r="A104" s="27"/>
+    <row r="102" spans="1:3" ht="14.25">
+      <c r="A102" s="27"/>
+      <c r="B102" s="61">
+        <v>84</v>
+      </c>
+      <c r="C102" s="66" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="51">
+      <c r="A103" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B103" s="66" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C103" s="71"/>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="12"/>
       <c r="B104" s="61">
-        <v>84</v>
-      </c>
-      <c r="C104" s="66" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="51">
-      <c r="A105" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B105" s="66" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C105" s="71"/>
+        <v>85</v>
+      </c>
+      <c r="C104" s="57" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="38.25">
+      <c r="A105" s="12"/>
+      <c r="B105" s="61">
+        <v>86</v>
+      </c>
+      <c r="C105" s="65" t="s">
+        <v>1119</v>
+      </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="12"/>
       <c r="B106" s="61">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C106" s="57" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="38.25">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="14.25">
       <c r="A107" s="12"/>
       <c r="B107" s="61">
-        <v>86</v>
-      </c>
-      <c r="C107" s="65" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <v>88</v>
+      </c>
+      <c r="C107" s="66" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="14.25">
       <c r="A108" s="12"/>
       <c r="B108" s="61">
-        <v>87</v>
-      </c>
-      <c r="C108" s="57" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="14.25">
-      <c r="A109" s="12"/>
-      <c r="B109" s="61">
-        <v>88</v>
-      </c>
-      <c r="C109" s="66" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="14.25">
-      <c r="A110" s="12"/>
+        <v>89</v>
+      </c>
+      <c r="C108" s="66" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B109" s="62" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C109" s="71"/>
+    </row>
+    <row r="110" spans="1:3">
       <c r="B110" s="61">
-        <v>89</v>
-      </c>
-      <c r="C110" s="66" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B111" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="C110" s="62" t="s">
         <v>1120</v>
       </c>
-      <c r="C111" s="71"/>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="B112" s="61">
-        <v>90</v>
-      </c>
-      <c r="C112" s="62" t="s">
-        <v>1120</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10585,16 +10567,16 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="54.75" thickBot="1">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="77" t="s">
+      <c r="D16" s="78" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="78" t="s">
         <v>229</v>
       </c>
       <c r="J16" s="48" t="s">
@@ -10623,10 +10605,10 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="68.25" thickBot="1">
-      <c r="A17" s="74"/>
-      <c r="B17" s="75"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="77"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
       <c r="J17" s="48" t="s">
         <v>982</v>
       </c>
@@ -10653,10 +10635,10 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="39" thickBot="1">
-      <c r="A18" s="74"/>
-      <c r="B18" s="75"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
+      <c r="A18" s="76"/>
+      <c r="B18" s="77"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
       <c r="J18" s="48" t="s">
         <v>984</v>
       </c>

</xml_diff>